<commit_message>
Fixed issues with surveillance quality indicators
</commit_message>
<xml_diff>
--- a/src/Data/country_data_LAC.xlsx
+++ b/src/Data/country_data_LAC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/mr-risk-assessment-regional/src/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{692A1575-60CA-4A50-B5C4-08F2C4750E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06363304-D986-4598-9D5E-C462A0E2FFEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFF9321E-16BB-4D2B-BBE8-791DE1528652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="773" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="773" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -3038,8 +3038,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="A2:D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3049,7 +3049,9 @@
     <col min="4" max="4" width="24.453125" style="27" customWidth="1"/>
     <col min="5" max="5" width="20.453125" style="27" customWidth="1"/>
     <col min="6" max="6" width="27.81640625" style="27" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="27"/>
+    <col min="7" max="8" width="9.1796875" style="27"/>
+    <col min="9" max="9" width="9.81640625" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="45" customHeight="1">
@@ -3086,7 +3088,7 @@
         <v>127</v>
       </c>
       <c r="E2" s="43">
-        <v>45696.159</v>
+        <v>45696159</v>
       </c>
       <c r="F2" s="43">
         <v>3123228.753</v>
@@ -3106,7 +3108,7 @@
         <v>130</v>
       </c>
       <c r="E3" s="43">
-        <v>12413.315000000001</v>
+        <v>12413315</v>
       </c>
       <c r="F3" s="43">
         <v>1138583.46</v>
@@ -3126,7 +3128,7 @@
         <v>131</v>
       </c>
       <c r="E4" s="43">
-        <v>211998.573</v>
+        <v>211998573</v>
       </c>
       <c r="F4" s="43">
         <v>9114834.9829999991</v>
@@ -3146,7 +3148,7 @@
         <v>132</v>
       </c>
       <c r="E5" s="43">
-        <v>19764.771000000001</v>
+        <v>19764771</v>
       </c>
       <c r="F5" s="43">
         <v>909611.86</v>
@@ -3166,7 +3168,7 @@
         <v>133</v>
       </c>
       <c r="E6" s="43">
-        <v>52886.362999999998</v>
+        <v>52886363</v>
       </c>
       <c r="F6" s="43">
         <v>1150064.807</v>
@@ -3186,7 +3188,7 @@
         <v>136</v>
       </c>
       <c r="E7" s="43">
-        <v>5129.91</v>
+        <v>5129910</v>
       </c>
       <c r="F7" s="43">
         <v>51602.983999999997</v>
@@ -3206,7 +3208,7 @@
         <v>139</v>
       </c>
       <c r="E8" s="43">
-        <v>10979.782999999999</v>
+        <v>10979783</v>
       </c>
       <c r="F8" s="43">
         <v>116600.95699999999</v>
@@ -3226,7 +3228,7 @@
         <v>140</v>
       </c>
       <c r="E9" s="43">
-        <v>11427.557000000001</v>
+        <v>11427557</v>
       </c>
       <c r="F9" s="43">
         <v>48450.534</v>
@@ -3246,7 +3248,7 @@
         <v>141</v>
       </c>
       <c r="E10" s="43">
-        <v>18135.477999999999</v>
+        <v>18135478</v>
       </c>
       <c r="F10" s="43">
         <v>255858.46</v>
@@ -3266,7 +3268,7 @@
         <v>142</v>
       </c>
       <c r="E11" s="43">
-        <v>18406.359</v>
+        <v>18406359</v>
       </c>
       <c r="F11" s="43">
         <v>109318.325</v>
@@ -3286,7 +3288,7 @@
         <v>143</v>
       </c>
       <c r="E12" s="43">
-        <v>10825.703</v>
+        <v>10825703</v>
       </c>
       <c r="F12" s="43">
         <v>113740.012</v>
@@ -3306,7 +3308,7 @@
         <v>144</v>
       </c>
       <c r="E13" s="43">
-        <v>11772.557000000001</v>
+        <v>11772557</v>
       </c>
       <c r="F13" s="43">
         <v>26596.12</v>
@@ -3326,7 +3328,7 @@
         <v>145</v>
       </c>
       <c r="E14" s="43">
-        <v>130861.007</v>
+        <v>130861007</v>
       </c>
       <c r="F14" s="43">
         <v>2041404.0209999999</v>
@@ -3346,7 +3348,7 @@
         <v>146</v>
       </c>
       <c r="E15" s="43">
-        <v>6916.14</v>
+        <v>6916140</v>
       </c>
       <c r="F15" s="43">
         <v>121093.95299999999</v>
@@ -3366,7 +3368,7 @@
         <v>147</v>
       </c>
       <c r="E16" s="43">
-        <v>4515.5770000000002</v>
+        <v>4515577</v>
       </c>
       <c r="F16" s="43">
         <v>75762.41</v>
@@ -3386,7 +3388,7 @@
         <v>148</v>
       </c>
       <c r="E17" s="43">
-        <v>34217.847999999998</v>
+        <v>34217848</v>
       </c>
       <c r="F17" s="43">
         <v>1320174.4839999999</v>
@@ -3406,7 +3408,7 @@
         <v>149</v>
       </c>
       <c r="E18" s="43">
-        <v>6929.1530000000002</v>
+        <v>6929153</v>
       </c>
       <c r="F18" s="43">
         <v>433561.51500000001</v>
@@ -3426,7 +3428,7 @@
         <v>150</v>
       </c>
       <c r="E19" s="43">
-        <v>6338.1930000000002</v>
+        <v>6338193</v>
       </c>
       <c r="F19" s="43">
         <v>20769.637999999999</v>
@@ -3446,7 +3448,7 @@
         <v>151</v>
       </c>
       <c r="E20" s="43">
-        <v>3386.59</v>
+        <v>3386590</v>
       </c>
       <c r="F20" s="43">
         <v>199021.40299999999</v>
@@ -3466,7 +3468,7 @@
         <v>152</v>
       </c>
       <c r="E21" s="43">
-        <v>28405.543000000001</v>
+        <v>28405543</v>
       </c>
       <c r="F21" s="43">
         <v>927152.6</v>
@@ -3485,7 +3487,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="A3:D22"/>
     </sheetView>
   </sheetViews>
@@ -7652,8 +7654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAE9CC2-3F53-41DA-8603-00D488002387}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>

</xml_diff>